<commit_message>
Finishing up the project
- Minor refactor
- Hide some unnessessary  funtion
</commit_message>
<xml_diff>
--- a/App/template/Báo giá QTSC.xlsx
+++ b/App/template/Báo giá QTSC.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Project\Study\ExcelTemplateRenderer\App\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -69,9 +69,6 @@
     <t>Công ty QTSC xin trân trọng báo giá {{categoryGroup}}  như sau:</t>
   </si>
   <si>
-    <t>{% if discount == 0 %}- Báo giá này sẽ áp dụng chính sách giảm giá {{discount}} %{% endif %}</t>
-  </si>
-  <si>
     <t>- Giá trên chưa bao gồm thuế {{tax}} % VAT</t>
   </si>
   <si>
@@ -88,6 +85,9 @@
   </si>
   <si>
     <t>{% for item in items %}</t>
+  </si>
+  <si>
+    <t>{% if discount != 0 %}- Báo giá này sẽ áp dụng chính sách giảm giá {{discount}} %{% endif %}</t>
   </si>
 </sst>
 </file>
@@ -251,52 +251,46 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -306,13 +300,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -696,7 +696,7 @@
   <dimension ref="A2:AH22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -707,390 +707,385 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
-      <c r="U2" s="2"/>
-      <c r="V2" s="2"/>
-      <c r="W2" s="2"/>
-      <c r="X2" s="2"/>
-      <c r="Y2" s="2"/>
-      <c r="Z2" s="2"/>
-      <c r="AA2" s="2"/>
-      <c r="AB2" s="2"/>
-      <c r="AC2" s="2"/>
-      <c r="AD2" s="2"/>
-      <c r="AE2" s="2"/>
-      <c r="AF2" s="2"/>
-      <c r="AG2" s="2"/>
-      <c r="AH2" s="3"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="22"/>
+      <c r="Q2" s="22"/>
+      <c r="R2" s="22"/>
+      <c r="S2" s="22"/>
+      <c r="T2" s="22"/>
+      <c r="U2" s="22"/>
+      <c r="V2" s="22"/>
+      <c r="W2" s="22"/>
+      <c r="X2" s="22"/>
+      <c r="Y2" s="22"/>
+      <c r="Z2" s="22"/>
+      <c r="AA2" s="22"/>
+      <c r="AB2" s="22"/>
+      <c r="AC2" s="22"/>
+      <c r="AD2" s="22"/>
+      <c r="AE2" s="22"/>
+      <c r="AF2" s="22"/>
+      <c r="AG2" s="22"/>
+      <c r="AH2" s="2"/>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
-      <c r="V3" s="2"/>
-      <c r="W3" s="2"/>
-      <c r="X3" s="2"/>
-      <c r="Y3" s="2"/>
-      <c r="Z3" s="2"/>
-      <c r="AA3" s="2"/>
-      <c r="AB3" s="2"/>
-      <c r="AC3" s="2"/>
-      <c r="AD3" s="2"/>
-      <c r="AE3" s="2"/>
-      <c r="AF3" s="2"/>
-      <c r="AG3" s="2"/>
-      <c r="AH3" s="3"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22"/>
+      <c r="N3" s="22"/>
+      <c r="O3" s="22"/>
+      <c r="P3" s="22"/>
+      <c r="Q3" s="22"/>
+      <c r="R3" s="22"/>
+      <c r="S3" s="22"/>
+      <c r="T3" s="22"/>
+      <c r="U3" s="22"/>
+      <c r="V3" s="22"/>
+      <c r="W3" s="22"/>
+      <c r="X3" s="22"/>
+      <c r="Y3" s="22"/>
+      <c r="Z3" s="22"/>
+      <c r="AA3" s="22"/>
+      <c r="AB3" s="22"/>
+      <c r="AC3" s="22"/>
+      <c r="AD3" s="22"/>
+      <c r="AE3" s="22"/>
+      <c r="AF3" s="22"/>
+      <c r="AG3" s="22"/>
+      <c r="AH3" s="2"/>
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="L4" s="4" t="s">
+      <c r="L4" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="4"/>
-      <c r="S4" s="4"/>
-      <c r="T4" s="4"/>
-      <c r="U4" s="4"/>
-      <c r="V4" s="4"/>
-      <c r="W4" s="4"/>
-      <c r="X4" s="4"/>
-      <c r="Y4" s="4"/>
-      <c r="Z4" s="4"/>
-      <c r="AA4" s="4"/>
-      <c r="AB4" s="4"/>
-      <c r="AC4" s="4"/>
-      <c r="AD4" s="4"/>
-      <c r="AE4" s="4"/>
-      <c r="AF4" s="4"/>
-      <c r="AG4" s="4"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="23"/>
+      <c r="O4" s="23"/>
+      <c r="P4" s="23"/>
+      <c r="Q4" s="23"/>
+      <c r="R4" s="23"/>
+      <c r="S4" s="23"/>
+      <c r="T4" s="23"/>
+      <c r="U4" s="23"/>
+      <c r="V4" s="23"/>
+      <c r="W4" s="23"/>
+      <c r="X4" s="23"/>
+      <c r="Y4" s="23"/>
+      <c r="Z4" s="23"/>
+      <c r="AA4" s="23"/>
+      <c r="AB4" s="23"/>
+      <c r="AC4" s="23"/>
+      <c r="AD4" s="23"/>
+      <c r="AE4" s="23"/>
+      <c r="AF4" s="23"/>
+      <c r="AG4" s="23"/>
     </row>
     <row r="8" spans="1:34" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="5"/>
-      <c r="R8" s="5"/>
-      <c r="S8" s="5"/>
-      <c r="T8" s="5"/>
-      <c r="U8" s="5"/>
-      <c r="V8" s="5"/>
-      <c r="W8" s="5"/>
-      <c r="X8" s="5"/>
-      <c r="Y8" s="5"/>
-      <c r="Z8" s="5"/>
-      <c r="AA8" s="5"/>
-      <c r="AB8" s="5"/>
-      <c r="AC8" s="5"/>
-      <c r="AD8" s="5"/>
-      <c r="AE8" s="5"/>
-      <c r="AF8" s="5"/>
-      <c r="AG8" s="5"/>
-      <c r="AH8" s="6"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="24"/>
+      <c r="N8" s="24"/>
+      <c r="O8" s="24"/>
+      <c r="P8" s="24"/>
+      <c r="Q8" s="24"/>
+      <c r="R8" s="24"/>
+      <c r="S8" s="24"/>
+      <c r="T8" s="24"/>
+      <c r="U8" s="24"/>
+      <c r="V8" s="24"/>
+      <c r="W8" s="24"/>
+      <c r="X8" s="24"/>
+      <c r="Y8" s="24"/>
+      <c r="Z8" s="24"/>
+      <c r="AA8" s="24"/>
+      <c r="AB8" s="24"/>
+      <c r="AC8" s="24"/>
+      <c r="AD8" s="24"/>
+      <c r="AE8" s="24"/>
+      <c r="AF8" s="24"/>
+      <c r="AG8" s="24"/>
+      <c r="AH8" s="3"/>
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="7"/>
-      <c r="Q10" s="7"/>
-      <c r="R10" s="7"/>
-      <c r="S10" s="7"/>
-      <c r="T10" s="7"/>
-      <c r="U10" s="7"/>
-      <c r="V10" s="7"/>
-      <c r="W10" s="7"/>
-      <c r="X10" s="7"/>
-      <c r="Y10" s="7"/>
-      <c r="Z10" s="7"/>
-      <c r="AA10" s="7"/>
-      <c r="AB10" s="7"/>
-      <c r="AC10" s="7"/>
-      <c r="AD10" s="7"/>
-      <c r="AE10" s="7"/>
-      <c r="AF10" s="7"/>
-      <c r="AG10" s="7"/>
-      <c r="AH10" s="8"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="25"/>
+      <c r="L10" s="25"/>
+      <c r="M10" s="25"/>
+      <c r="N10" s="25"/>
+      <c r="O10" s="25"/>
+      <c r="P10" s="25"/>
+      <c r="Q10" s="25"/>
+      <c r="R10" s="25"/>
+      <c r="S10" s="25"/>
+      <c r="T10" s="25"/>
+      <c r="U10" s="25"/>
+      <c r="V10" s="25"/>
+      <c r="W10" s="25"/>
+      <c r="X10" s="25"/>
+      <c r="Y10" s="25"/>
+      <c r="Z10" s="25"/>
+      <c r="AA10" s="25"/>
+      <c r="AB10" s="25"/>
+      <c r="AC10" s="25"/>
+      <c r="AD10" s="25"/>
+      <c r="AE10" s="25"/>
+      <c r="AF10" s="25"/>
+      <c r="AG10" s="25"/>
+      <c r="AH10" s="4"/>
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9"/>
-      <c r="N12" s="9"/>
-      <c r="O12" s="9"/>
-      <c r="P12" s="9"/>
-      <c r="Q12" s="9"/>
-      <c r="R12" s="9"/>
-      <c r="S12" s="9"/>
-      <c r="T12" s="9"/>
-      <c r="U12" s="9"/>
-      <c r="V12" s="9"/>
-      <c r="W12" s="9"/>
-      <c r="X12" s="9"/>
-      <c r="Y12" s="9"/>
-      <c r="Z12" s="9"/>
-      <c r="AA12" s="9"/>
-      <c r="AB12" s="9"/>
-      <c r="AC12" s="9"/>
-      <c r="AD12" s="9"/>
-      <c r="AE12" s="9"/>
-      <c r="AF12" s="9"/>
-      <c r="AG12" s="9"/>
-      <c r="AH12" s="10"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="26"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="26"/>
+      <c r="L12" s="26"/>
+      <c r="M12" s="26"/>
+      <c r="N12" s="26"/>
+      <c r="O12" s="26"/>
+      <c r="P12" s="26"/>
+      <c r="Q12" s="26"/>
+      <c r="R12" s="26"/>
+      <c r="S12" s="26"/>
+      <c r="T12" s="26"/>
+      <c r="U12" s="26"/>
+      <c r="V12" s="26"/>
+      <c r="W12" s="26"/>
+      <c r="X12" s="26"/>
+      <c r="Y12" s="26"/>
+      <c r="Z12" s="26"/>
+      <c r="AA12" s="26"/>
+      <c r="AB12" s="26"/>
+      <c r="AC12" s="26"/>
+      <c r="AD12" s="26"/>
+      <c r="AE12" s="26"/>
+      <c r="AF12" s="26"/>
+      <c r="AG12" s="26"/>
+      <c r="AH12" s="5"/>
     </row>
     <row r="13" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:34" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="21" t="s">
+      <c r="C14" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="22"/>
-      <c r="J14" s="22"/>
-      <c r="K14" s="22"/>
-      <c r="L14" s="22"/>
-      <c r="M14" s="22"/>
-      <c r="N14" s="22"/>
-      <c r="O14" s="22"/>
-      <c r="P14" s="22"/>
-      <c r="Q14" s="22"/>
-      <c r="R14" s="22"/>
-      <c r="S14" s="22"/>
-      <c r="T14" s="22"/>
-      <c r="U14" s="23"/>
-      <c r="V14" s="12" t="s">
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="20"/>
+      <c r="N14" s="20"/>
+      <c r="O14" s="20"/>
+      <c r="P14" s="20"/>
+      <c r="Q14" s="20"/>
+      <c r="R14" s="20"/>
+      <c r="S14" s="20"/>
+      <c r="T14" s="20"/>
+      <c r="U14" s="21"/>
+      <c r="V14" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="W14" s="13"/>
-      <c r="X14" s="13"/>
-      <c r="Y14" s="13"/>
-      <c r="Z14" s="13"/>
-      <c r="AA14" s="13"/>
-      <c r="AB14" s="13"/>
-      <c r="AC14" s="14"/>
-      <c r="AD14" s="12" t="s">
+      <c r="W14" s="17"/>
+      <c r="X14" s="17"/>
+      <c r="Y14" s="17"/>
+      <c r="Z14" s="17"/>
+      <c r="AA14" s="17"/>
+      <c r="AB14" s="17"/>
+      <c r="AC14" s="18"/>
+      <c r="AD14" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="AE14" s="13"/>
-      <c r="AF14" s="13"/>
-      <c r="AG14" s="14"/>
-      <c r="AH14" s="15"/>
+      <c r="AE14" s="17"/>
+      <c r="AF14" s="17"/>
+      <c r="AG14" s="18"/>
+      <c r="AH14" s="7"/>
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="12"/>
+      <c r="P15" s="12"/>
+      <c r="Q15" s="12"/>
+      <c r="R15" s="12"/>
+      <c r="S15" s="12"/>
+      <c r="T15" s="12"/>
+      <c r="U15" s="12"/>
+      <c r="V15" s="12"/>
+      <c r="W15" s="12"/>
+      <c r="X15" s="12"/>
+      <c r="Y15" s="12"/>
+      <c r="Z15" s="12"/>
+      <c r="AA15" s="12"/>
+      <c r="AB15" s="12"/>
+      <c r="AC15" s="12"/>
+      <c r="AD15" s="12"/>
+      <c r="AE15" s="12"/>
+      <c r="AF15" s="12"/>
+      <c r="AG15" s="12"/>
+    </row>
+    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="B16" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="14"/>
+      <c r="O16" s="14"/>
+      <c r="P16" s="14"/>
+      <c r="Q16" s="14"/>
+      <c r="R16" s="14"/>
+      <c r="S16" s="14"/>
+      <c r="T16" s="14"/>
+      <c r="U16" s="14"/>
+      <c r="V16" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="W16" s="15"/>
+      <c r="X16" s="15"/>
+      <c r="Y16" s="15"/>
+      <c r="Z16" s="15"/>
+      <c r="AA16" s="15"/>
+      <c r="AB16" s="15"/>
+      <c r="AC16" s="15"/>
+      <c r="AD16" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="AE16" s="15"/>
+      <c r="AF16" s="15"/>
+      <c r="AG16" s="15"/>
+    </row>
+    <row r="17" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B17" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="13"/>
+      <c r="O17" s="13"/>
+      <c r="P17" s="13"/>
+      <c r="Q17" s="13"/>
+      <c r="R17" s="13"/>
+      <c r="S17" s="13"/>
+      <c r="T17" s="13"/>
+      <c r="U17" s="13"/>
+      <c r="V17" s="13"/>
+      <c r="W17" s="13"/>
+      <c r="X17" s="13"/>
+      <c r="Y17" s="13"/>
+      <c r="Z17" s="13"/>
+      <c r="AA17" s="13"/>
+      <c r="AB17" s="13"/>
+      <c r="AC17" s="13"/>
+      <c r="AD17" s="13"/>
+      <c r="AE17" s="13"/>
+      <c r="AF17" s="13"/>
+      <c r="AG17" s="13"/>
+    </row>
+    <row r="18" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B18" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="C19" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="C20" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="16"/>
-      <c r="L15" s="16"/>
-      <c r="M15" s="16"/>
-      <c r="N15" s="16"/>
-      <c r="O15" s="16"/>
-      <c r="P15" s="16"/>
-      <c r="Q15" s="16"/>
-      <c r="R15" s="16"/>
-      <c r="S15" s="16"/>
-      <c r="T15" s="16"/>
-      <c r="U15" s="16"/>
-      <c r="V15" s="16"/>
-      <c r="W15" s="16"/>
-      <c r="X15" s="16"/>
-      <c r="Y15" s="16"/>
-      <c r="Z15" s="16"/>
-      <c r="AA15" s="16"/>
-      <c r="AB15" s="16"/>
-      <c r="AC15" s="16"/>
-      <c r="AD15" s="16"/>
-      <c r="AE15" s="16"/>
-      <c r="AF15" s="16"/>
-      <c r="AG15" s="16"/>
-    </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="B16" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="25"/>
-      <c r="I16" s="25"/>
-      <c r="J16" s="25"/>
-      <c r="K16" s="25"/>
-      <c r="L16" s="25"/>
-      <c r="M16" s="25"/>
-      <c r="N16" s="25"/>
-      <c r="O16" s="25"/>
-      <c r="P16" s="25"/>
-      <c r="Q16" s="25"/>
-      <c r="R16" s="25"/>
-      <c r="S16" s="25"/>
-      <c r="T16" s="25"/>
-      <c r="U16" s="25"/>
-      <c r="V16" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="W16" s="26"/>
-      <c r="X16" s="26"/>
-      <c r="Y16" s="26"/>
-      <c r="Z16" s="26"/>
-      <c r="AA16" s="26"/>
-      <c r="AB16" s="26"/>
-      <c r="AC16" s="26"/>
-      <c r="AD16" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="AE16" s="26"/>
-      <c r="AF16" s="26"/>
-      <c r="AG16" s="26"/>
-    </row>
-    <row r="17" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B17" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="17"/>
-      <c r="M17" s="17"/>
-      <c r="N17" s="17"/>
-      <c r="O17" s="17"/>
-      <c r="P17" s="17"/>
-      <c r="Q17" s="17"/>
-      <c r="R17" s="17"/>
-      <c r="S17" s="17"/>
-      <c r="T17" s="17"/>
-      <c r="U17" s="17"/>
-      <c r="V17" s="17"/>
-      <c r="W17" s="17"/>
-      <c r="X17" s="17"/>
-      <c r="Y17" s="17"/>
-      <c r="Z17" s="17"/>
-      <c r="AA17" s="17"/>
-      <c r="AB17" s="17"/>
-      <c r="AC17" s="17"/>
-      <c r="AD17" s="17"/>
-      <c r="AE17" s="17"/>
-      <c r="AF17" s="17"/>
-      <c r="AG17" s="17"/>
-    </row>
-    <row r="18" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B18" s="18" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="C19" s="19" t="s">
+    </row>
+    <row r="21" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B21" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B22" s="10" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="20" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="C20" s="19" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B21" s="20" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B22" s="20" t="s">
+      <c r="P22" s="10" t="s">
         <v>16</v>
-      </c>
-      <c r="P22" s="20" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B15:AG15"/>
-    <mergeCell ref="B17:AG17"/>
-    <mergeCell ref="C16:U16"/>
-    <mergeCell ref="AD16:AG16"/>
-    <mergeCell ref="V16:AC16"/>
     <mergeCell ref="AD14:AG14"/>
     <mergeCell ref="C14:U14"/>
     <mergeCell ref="L2:AG3"/>
@@ -1099,6 +1094,11 @@
     <mergeCell ref="A8:AG8"/>
     <mergeCell ref="A10:AG10"/>
     <mergeCell ref="A12:AG12"/>
+    <mergeCell ref="B15:AG15"/>
+    <mergeCell ref="B17:AG17"/>
+    <mergeCell ref="C16:U16"/>
+    <mergeCell ref="AD16:AG16"/>
+    <mergeCell ref="V16:AC16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>